<commit_message>
Implemented Testcase02, Testcase03, Testcase04
</commit_message>
<xml_diff>
--- a/app/src/test/resources/qtripTestDataSet.xlsx
+++ b/app/src/test/resources/qtripTestDataSet.xlsx
@@ -4,10 +4,13 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9000"/>
+    <workbookView windowWidth="23040" windowHeight="9000" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="TC01" sheetId="1" r:id="rId1"/>
+    <sheet name="TC02" sheetId="2" r:id="rId2"/>
+    <sheet name="TC03" sheetId="3" r:id="rId3"/>
+    <sheet name="TC04" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="77">
   <si>
     <t>#</t>
   </si>
@@ -66,6 +69,198 @@
   </si>
   <si>
     <t>PassDTeam0101</t>
+  </si>
+  <si>
+    <t>cityName</t>
+  </si>
+  <si>
+    <t>categoryFilter</t>
+  </si>
+  <si>
+    <t>durationFilter</t>
+  </si>
+  <si>
+    <t>expectedFilteredResults</t>
+  </si>
+  <si>
+    <t>expectedUnfilteredResults</t>
+  </si>
+  <si>
+    <t>Bengaluru</t>
+  </si>
+  <si>
+    <t>Cycling Routes</t>
+  </si>
+  <si>
+    <t>6-12 Hours</t>
+  </si>
+  <si>
+    <t>Singapore</t>
+  </si>
+  <si>
+    <t>Hillside Getaways</t>
+  </si>
+  <si>
+    <t>Goa</t>
+  </si>
+  <si>
+    <t>Party Spots</t>
+  </si>
+  <si>
+    <t>2-6 Hours</t>
+  </si>
+  <si>
+    <t>Paris</t>
+  </si>
+  <si>
+    <t>Serene Beaches</t>
+  </si>
+  <si>
+    <t>12+ Hours</t>
+  </si>
+  <si>
+    <t>Malaysia</t>
+  </si>
+  <si>
+    <t>newUserName</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>searchCity</t>
+  </si>
+  <si>
+    <t>adventureName</t>
+  </si>
+  <si>
+    <t>guestName</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t>user01@gmail.com</t>
+  </si>
+  <si>
+    <t>qwertyuiop</t>
+  </si>
+  <si>
+    <t>Niaboytown</t>
+  </si>
+  <si>
+    <t>palam</t>
+  </si>
+  <si>
+    <t>16-11-2025</t>
+  </si>
+  <si>
+    <t>user02@gmail.com</t>
+  </si>
+  <si>
+    <t>asdfghjkl</t>
+  </si>
+  <si>
+    <t>Grand Ashland</t>
+  </si>
+  <si>
+    <t>biden</t>
+  </si>
+  <si>
+    <t>26-11-2025</t>
+  </si>
+  <si>
+    <t>user03@gmail.com</t>
+  </si>
+  <si>
+    <t>zxcvbnm</t>
+  </si>
+  <si>
+    <t>Bangkok</t>
+  </si>
+  <si>
+    <t>Tifwales Ferry</t>
+  </si>
+  <si>
+    <t>prabhu</t>
+  </si>
+  <si>
+    <t>26-12-2025</t>
+  </si>
+  <si>
+    <t>user04@gmail.com</t>
+  </si>
+  <si>
+    <t>qazwsx</t>
+  </si>
+  <si>
+    <t>Lia</t>
+  </si>
+  <si>
+    <t>Thton</t>
+  </si>
+  <si>
+    <t>28-12-2025</t>
+  </si>
+  <si>
+    <t>user05@gmail.com</t>
+  </si>
+  <si>
+    <t>plmokn</t>
+  </si>
+  <si>
+    <t>Kenntic End</t>
+  </si>
+  <si>
+    <t>Cha</t>
+  </si>
+  <si>
+    <t>31-12-2025</t>
+  </si>
+  <si>
+    <t>newUsername</t>
+  </si>
+  <si>
+    <t>dataSet01</t>
+  </si>
+  <si>
+    <t>dataSet02</t>
+  </si>
+  <si>
+    <t>dataSet03</t>
+  </si>
+  <si>
+    <t>Bengaluru;Niaboytown;Chicky;01-01-2025;2</t>
+  </si>
+  <si>
+    <t>Kolkata;Thton;Cha Cha;01-02-2025;3</t>
+  </si>
+  <si>
+    <t>Malaysia;Wootkentree;Bom Bom;02-12-2025;1</t>
+  </si>
+  <si>
+    <t>Bengaluru;Fort Sionnnn;Chicky;01-01-2025;2</t>
+  </si>
+  <si>
+    <t>Kolkata;North Gelgoon;Cha Cha;01-02-2025;3</t>
+  </si>
+  <si>
+    <t>Malaysia;Wootkentree;Lya;02-12-2025;1</t>
+  </si>
+  <si>
+    <t>Goa;Perthby;Chicky;01-01-2025;2</t>
+  </si>
+  <si>
+    <t>Bengaluru;Fort Sion;Chicky;01-01-2025;2</t>
+  </si>
+  <si>
+    <t>qwaszxedc</t>
+  </si>
+  <si>
+    <t>polkmnijn</t>
   </si>
 </sst>
 </file>
@@ -105,7 +300,7 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -113,7 +308,7 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -571,12 +766,12 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -701,18 +896,26 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1036,15 +1239,16 @@
   <sheetPr/>
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="5" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="3.66666666666667" style="1" customWidth="1"/>
-    <col min="2" max="3" width="50.7777777777778" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="9" style="2"/>
+    <col min="1" max="1" width="2.66666666666667" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.2222222222222" style="7" customWidth="1"/>
+    <col min="3" max="3" width="15.6666666666667" style="7" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="7"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:3">
@@ -1062,10 +1266,10 @@
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="7" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1073,10 +1277,10 @@
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="7" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1084,10 +1288,10 @@
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="7" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1095,10 +1299,10 @@
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1106,10 +1310,10 @@
       <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="7" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1124,4 +1328,493 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="5" outlineLevelCol="5"/>
+  <cols>
+    <col min="1" max="1" width="2.66666666666667" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.77777777777778" style="7" customWidth="1"/>
+    <col min="3" max="3" width="16.6666666666667" style="7" customWidth="1"/>
+    <col min="4" max="4" width="13.4444444444444" style="7" customWidth="1"/>
+    <col min="5" max="5" width="22.8888888888889" style="7" customWidth="1"/>
+    <col min="6" max="6" width="25.4444444444444" style="7" customWidth="1"/>
+    <col min="7" max="16384" width="8.88888888888889" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="1:6">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="7">
+        <v>1</v>
+      </c>
+      <c r="F2" s="7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="7">
+        <v>1</v>
+      </c>
+      <c r="F3" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="7">
+        <v>1</v>
+      </c>
+      <c r="F4" s="7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="7">
+        <v>3</v>
+      </c>
+      <c r="F5" s="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="7">
+        <v>0</v>
+      </c>
+      <c r="F6" s="7">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="5" outlineLevelCol="7"/>
+  <cols>
+    <col min="1" max="1" width="2.66666666666667" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.2222222222222" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="4" max="4" width="10.4444444444444" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="6" max="6" width="11.4444444444444" customWidth="1"/>
+    <col min="7" max="7" width="11.1111111111111" customWidth="1"/>
+    <col min="8" max="8" width="6.55555555555556" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="1:8">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G4" t="s">
+        <v>52</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G5" t="s">
+        <v>57</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F6" t="s">
+        <v>61</v>
+      </c>
+      <c r="G6" t="s">
+        <v>62</v>
+      </c>
+      <c r="H6">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="user01@gmail.com"/>
+    <hyperlink ref="B3" r:id="rId2" display="user02@gmail.com"/>
+    <hyperlink ref="B4" r:id="rId3" display="user03@gmail.com"/>
+    <hyperlink ref="B5" r:id="rId4" display="user04@gmail.com"/>
+    <hyperlink ref="B6" r:id="rId5" display="user05@gmail.com"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="5" outlineLevelCol="5"/>
+  <cols>
+    <col min="1" max="1" width="2.66666666666667" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.2222222222222" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11" style="2" customWidth="1"/>
+    <col min="4" max="4" width="41.2222222222222" style="2" customWidth="1"/>
+    <col min="5" max="5" width="42.6666666666667" style="2" customWidth="1"/>
+    <col min="6" max="6" width="44.1111111111111" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="8.88888888888889" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="1:6">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="user01@gmail.com"/>
+    <hyperlink ref="B3" r:id="rId2" display="user02@gmail.com"/>
+    <hyperlink ref="B4" r:id="rId3" display="user03@gmail.com"/>
+    <hyperlink ref="B5" r:id="rId4" display="user04@gmail.com"/>
+    <hyperlink ref="B6" r:id="rId5" display="user05@gmail.com"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>